<commit_message>
Added Castiblando & Wilches research project. reference secitions with footnotesize fonts
</commit_message>
<xml_diff>
--- a/data/supervision_pre_en.xlsx
+++ b/data/supervision_pre_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E22E62-2231-4197-8D2D-43F0B8DE40E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4152EA7C-78FE-49BB-B229-20D93DA9012B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="supervision" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="59">
   <si>
     <t>what</t>
   </si>
@@ -201,6 +201,15 @@
   </si>
   <si>
     <t>Research project \textbf{\textit{(Distinction)}}: \textit{\href{http://hdl.handle.net/20.500.12209/10443}{Musicalidad y cohesión social: una aproximación experimental y bibliográfica desde el trabajo en equipo} [Musicality and social cohesion: An experimental and bibliographic approach from teamwork]}</t>
+  </si>
+  <si>
+    <t>2022 - 2023</t>
+  </si>
+  <si>
+    <t>Research project: \textit{\href{https://youtu.be/FlZvukFqTcc}{El rol del género en la identificación de la sociosexualidad a partir de las voces} [The role of gender in the identification of sociosexuality from voices]}</t>
+  </si>
+  <si>
+    <t>Maria Camila Wilches \&amp; Johan Sebatián Castiblanco</t>
   </si>
 </sst>
 </file>
@@ -1056,10 +1065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,24 +1141,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>58</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1157,47 +1166,47 @@
         <v>18</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
@@ -1205,84 +1214,84 @@
         <v>28</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+    <row r="12" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="3" t="s">
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="14" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1293,13 +1302,13 @@
         <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="60" x14ac:dyDescent="0.25">
@@ -1307,19 +1316,19 @@
         <v>28</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>28</v>
       </c>
@@ -1327,33 +1336,33 @@
         <v>24</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>28</v>
       </c>
@@ -1361,38 +1370,48 @@
         <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
@@ -1464,6 +1483,13 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Upd YouTube links for TPG3
</commit_message>
<xml_diff>
--- a/data/supervision_pre_en.xlsx
+++ b/data/supervision_pre_en.xlsx
@@ -43,35 +43,7 @@
     <t xml:space="preserve">2024 – 2025</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Juliana Pinzón Rodríguez </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">\&amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Valeria García Martínez</t>
-    </r>
+    <t xml:space="preserve">Juliana Pinzón Rodríguez \&amp; Valeria García Martínez</t>
   </si>
   <si>
     <t xml:space="preserve">\href{https://www.unbosque.edu.co/}{Universidad El Bosque}, Colombia</t>
@@ -116,13 +88,13 @@
     <t xml:space="preserve">Scharik Yuliana Bello Lizarazo, Maria Camila Plazas López \&amp; Natalia Rodríguez Bautista</t>
   </si>
   <si>
-    <t xml:space="preserve">Research project:  \textit{\href{https://youtu.be/Pb-00b41j98}{¿Es posible percibir la promiscuidad de una persona con tan solo escuchar su voz?} [Is it possible to perceive a person's promiscuity just by listening to his or her voice?]}</t>
+    <t xml:space="preserve">Research project:  \textit{\href{https://youtu.be/taKzODEX4zg}{¿Es posible percibir la promiscuidad de una persona con tan solo escuchar su voz?} [Is it possible to perceive a person's promiscuity just by listening to his or her voice?]}</t>
   </si>
   <si>
     <t xml:space="preserve">Isabella Russo</t>
   </si>
   <si>
-    <t xml:space="preserve">Research project:  \textit{\href{https://youtu.be/nX3p5Bt_vjQ}{¿El género, preferenca sexual y nivel de sociosexualidad de una persona podrían influir en su capacidad para detectar la sociosexualidad de otros a través de rostros?} [Could a person's gender, sexual preference and level of sociosexuality influence their ability to detect the sociosexuality of others from their faces?]}</t>
+    <t xml:space="preserve">Research project:  \textit{\href{https://youtu.be/RR7S5jRevsI}{¿El género, preferenca sexual y nivel de sociosexualidad de una persona podrían influir en su capacidad para detectar la sociosexualidad de otros a través de rostros?} [Could a person's gender, sexual preference and level of sociosexuality influence their ability to detect the sociosexuality of others from their faces?]}</t>
   </si>
   <si>
     <t xml:space="preserve">2022 - 2023</t>
@@ -131,7 +103,7 @@
     <t xml:space="preserve">Maria Camila Wilches \&amp; Johan Sebatián Castiblanco</t>
   </si>
   <si>
-    <t xml:space="preserve">Research project: \textit{\href{https://youtu.be/FlZvukFqTcc}{El rol del género en la identificación de la sociosexualidad a partir de las voces} [The role of gender in the identification of sociosexuality from voices]}</t>
+    <t xml:space="preserve">Research project: \textit{\href{https://youtu.be/NbPyhQAFlUk}{El rol del género en la identificación de la sociosexualidad a partir de las voces} [The role of gender in the identification of sociosexuality from voices]}</t>
   </si>
   <si>
     <t xml:space="preserve">2021 - 2022</t>
@@ -140,13 +112,13 @@
     <t xml:space="preserve">Angie Alejandra Lozano Sanjuan, Daniela Martínez Franco \&amp; Mariana Saavedra Botero  </t>
   </si>
   <si>
-    <t xml:space="preserve">Research project \textbf{\textit{(Distinction)}}: \textit{\href{https://youtu.be/A9xNV3BqRJw}{¿Somos capaces de detectar qué tan sociosexual es una persona a partir de su voz y/o su rostro?} [Are we able to detect the sociosexual orientation of a person from their voice and/or face?]}</t>
+    <t xml:space="preserve">Research project \textbf{\textit{(Distinction)}}: \textit{\href{https://youtu.be/xhYq7HeEPP4}{¿Somos capaces de detectar qué tan sociosexual es una persona a partir de su voz y/o su rostro?} [Are we able to detect the sociosexual orientation of a person from their voice and/or face?]}</t>
   </si>
   <si>
     <t xml:space="preserve">John Jairo Rubio </t>
   </si>
   <si>
-    <t xml:space="preserve">Research project: \textit{\href{https://youtu.be/G9eqxpyKF5A}{¿Existe relación entre la simetría facial y el atractivo de la voz?} [Association between facial symmetry and vocal attractiveness]}</t>
+    <t xml:space="preserve">Research project: \textit{\href{https://youtu.be/5o9Iea8VfDM}{¿Existe relación entre la simetría facial y el atractivo de la voz?} [Association between facial symmetry and vocal attractiveness]}</t>
   </si>
   <si>
     <t xml:space="preserve">2020 - 2021</t>
@@ -155,7 +127,7 @@
     <t xml:space="preserve">Maria Daniela Martínez Luna \&amp; Juan Sebastián Preciado Ruíz </t>
   </si>
   <si>
-    <t xml:space="preserve">Research project \textbf{\textit{(Distinction)}}: \textit{\href{https://youtu.be/BNNseX-PK7s}{¿Existe relación entre la sociosexualidad y la voz?} [Is there a relationship between sociosexuality and voice?]}</t>
+    <t xml:space="preserve">Research project \textbf{\textit{(Distinction)}}: \textit{\href{https://youtu.be/Ie07343LiIA}{¿Existe relación entre la sociosexualidad y la voz?} [Is there a relationship between sociosexuality and voice?]}</t>
   </si>
   <si>
     <t xml:space="preserve">2019 - 2021</t>
@@ -173,7 +145,7 @@
     <t xml:space="preserve">Danny Ferley Gaitan Rodríguez \&amp; Hasbleidy Gamboa Ordoñez </t>
   </si>
   <si>
-    <t xml:space="preserve">Research project: \textit{\href{https://youtu.be/J6nUuifYjbU}{Detección de infidelidad y sociosexualidad a partir de rostros: Análisis preliminar} [Perception of socio-sexuality from facial cues]}</t>
+    <t xml:space="preserve">Research project: \textit{\href{https://youtu.be/rkp2k_KzZsM}{Detección de infidelidad y sociosexualidad a partir de rostros: Análisis preliminar} [Perception of socio-sexuality from facial cues]}</t>
   </si>
   <si>
     <t xml:space="preserve">BA in Music Pedagogy</t>
@@ -270,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -291,12 +263,6 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -342,20 +308,24 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,517 +520,524 @@
   </sheetPr>
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="58.5703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="58.57421875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="78.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="67.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="74.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="78.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="67.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="74.86"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
+    <row r="5" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="1" t="s">
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="D8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="9" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1" t="s">
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="1" t="n">
+    <row r="10" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2" t="n">
         <v>2023</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="1" t="s">
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="11" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B12" s="1" t="s">
+    <row r="12" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" s="1" t="s">
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="1" t="s">
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" s="1" t="s">
+    <row r="15" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E15" s="1" t="s">
+      <c r="D15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="D16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+    <row r="17" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B18" s="1" t="s">
+    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="D18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+    <row r="19" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="D19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="20" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B21" s="1" t="s">
+    <row r="21" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="D21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="1" t="s">
+    <row r="22" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="D22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="23" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D23" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="1" t="s">
+      <c r="D23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B24" s="1" t="s">
+    <row r="24" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E24" s="1" t="s">
+      <c r="D24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B25" s="1" t="s">
+    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E25" s="1" t="s">
+      <c r="D25" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="1" t="s">
+    <row r="26" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="D26" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3"/>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
+      <c r="A33" s="4"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://hdl.handle.net/20.500.12495/18119"/>
+    <hyperlink ref="E3" r:id="rId1" display="Project: \textit{\href{https://hdl.handle.net/20.500.12495/18119}{Sociosexualidad percibida a partir del contenido verbal de los discursos} [Perceived sociosexuality based on speech verbal content]}"/>
+    <hyperlink ref="E9" r:id="rId2" display="https://youtu.be/taKzODEX4zg"/>
+    <hyperlink ref="E10" r:id="rId3" display="https://youtu.be/RR7S5jRevsI"/>
+    <hyperlink ref="E11" r:id="rId4" display="https://youtu.be/NbPyhQAFlUk"/>
+    <hyperlink ref="E12" r:id="rId5" display="https://youtu.be/xhYq7HeEPP4"/>
+    <hyperlink ref="E13" r:id="rId6" display="https://youtu.be/5o9Iea8VfDM"/>
+    <hyperlink ref="E14" r:id="rId7" display="https://youtu.be/Ie07343LiIA"/>
+    <hyperlink ref="E16" r:id="rId8" display="https://youtu.be/rkp2k_KzZsM"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>